<commit_message>
add invoice no check
</commit_message>
<xml_diff>
--- a/public/sample/consigner_bulk_import.xlsx
+++ b/public/sample/consigner_bulk_import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\easemylr-pro\public\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC025E8-53AB-451F-ACDC-66D45F12BFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AE2FED-133D-405E-86BA-7542E1D820DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0451C7E1-EA1E-46C7-BD19-57863157B07E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Sr No.</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>punjab</t>
-  </si>
-  <si>
-    <t>Location Id</t>
   </si>
   <si>
     <t>Regional Client Id</t>
@@ -495,121 +492,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75A53E2-04BB-4E8A-BEFF-EDEE00A6E289}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>8765435456</v>
       </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="M2" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="N2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P2">
+      <c r="O2">
         <v>160066</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{953050FB-A105-489E-A298-2FBDF9A455FD}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{953050FB-A105-489E-A298-2FBDF9A455FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>